<commit_message>
Update measure intensities figure
</commit_message>
<xml_diff>
--- a/figures/resources/measure_intensities.xlsx
+++ b/figures/resources/measure_intensities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tischer/Documents/training-resources/figures/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F02573A-F599-4048-B5F3-8B4C21F0697B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC1D378-3207-5041-9901-40A9656FE7C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12660" yWindow="6040" windowWidth="28040" windowHeight="15980" xr2:uid="{D567E1E8-8449-AE4B-9D00-1EA4643E292D}"/>
+    <workbookView xWindow="2220" yWindow="3500" windowWidth="28040" windowHeight="15980" xr2:uid="{D567E1E8-8449-AE4B-9D00-1EA4643E292D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,12 +66,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF37FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,17 +98,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF37FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -408,7 +427,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +458,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>85</v>
       </c>
       <c r="B2">
@@ -461,7 +480,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>171</v>
       </c>
       <c r="B3">

</xml_diff>